<commit_message>
Fixed bugs with AcronymSchema when entities get skipped
</commit_message>
<xml_diff>
--- a/input_data/2001/basic_posting_flows.big_rocks.burnout/brb_opus.FusionOpus.big-rocks.journeys.a6i.xlsx
+++ b/input_data/2001/basic_posting_flows.big_rocks.burnout/brb_opus.FusionOpus.big-rocks.journeys.a6i.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\knowledge_base\tests_integration\input_data\basic_posting_flows.big_rocks.burnout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\input_data\2001\basic_posting_flows.big_rocks.burnout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A5AA8-69E4-4364-AD85-6453FB67389D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB66BACC-8633-4306-A58C-72238889F75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>manifestAPI</t>
   </si>
@@ -241,19 +241,25 @@
     <t>sub rocks</t>
   </si>
   <si>
-    <t>B2:D10</t>
-  </si>
-  <si>
-    <t>E2:E10</t>
-  </si>
-  <si>
-    <t>G2:H8</t>
-  </si>
-  <si>
     <t>burnout</t>
   </si>
   <si>
     <t>knowledgeBase</t>
+  </si>
+  <si>
+    <t>Tiny rocks</t>
+  </si>
+  <si>
+    <t>API for a very specific case</t>
+  </si>
+  <si>
+    <t>F2:F11</t>
+  </si>
+  <si>
+    <t>B2:E11</t>
+  </si>
+  <si>
+    <t>H2:I9</t>
   </si>
 </sst>
 </file>
@@ -726,7 +732,7 @@
   <dimension ref="B1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -758,7 +764,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>26</v>
@@ -825,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -881,7 +887,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
@@ -905,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
@@ -929,7 +935,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
@@ -948,34 +954,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:I11"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="55.73046875" customWidth="1"/>
-    <col min="4" max="4" width="24.3984375" customWidth="1"/>
-    <col min="5" max="5" width="7.265625" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" customWidth="1"/>
-    <col min="8" max="9" width="12.86328125" customWidth="1"/>
+    <col min="4" max="5" width="24.3984375" customWidth="1"/>
+    <col min="6" max="6" width="7.265625" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" customWidth="1"/>
+    <col min="9" max="10" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
@@ -986,19 +992,22 @@
         <v>68</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
@@ -1006,173 +1015,196 @@
         <v>46</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="7">
+      <c r="E3" s="4"/>
+      <c r="F3" s="7">
         <v>4050</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="7">
         <v>3584</v>
       </c>
-      <c r="I3" s="8">
-        <f>SUM(H$3:H3)</f>
+      <c r="J3" s="8">
+        <f>SUM(I$3:I3)</f>
         <v>3584</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="7">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="7">
         <v>6600</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I5" s="7">
         <v>5207</v>
       </c>
-      <c r="I4" s="8">
-        <f>SUM(H$3:H4)</f>
+      <c r="J5" s="8">
+        <f>SUM(I$3:I5)</f>
         <v>8791</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="7">
         <v>4500</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I6" s="7">
         <v>5575</v>
       </c>
-      <c r="I5" s="8">
-        <f>SUM(H$3:H5)</f>
+      <c r="J6" s="8">
+        <f>SUM(I$3:I6)</f>
         <v>14366</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="G6" s="4" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I7" s="7">
         <v>5800</v>
       </c>
-      <c r="I6" s="8">
-        <f>SUM(H$3:H6)</f>
+      <c r="J7" s="8">
+        <f>SUM(I$3:I7)</f>
         <v>20166</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="7">
-        <v>5100</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="7">
-        <v>5860</v>
-      </c>
-      <c r="I7" s="8">
-        <f>SUM(H$3:H7)</f>
-        <v>26026</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7">
+        <v>5100</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5860</v>
+      </c>
+      <c r="J8" s="8">
+        <f>SUM(I$3:I8)</f>
+        <v>26026</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E9" s="4"/>
+      <c r="F9" s="7">
         <v>5250</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I9" s="7">
         <v>998</v>
       </c>
-      <c r="I8" s="8">
-        <f>SUM(H$3:H8)</f>
+      <c r="J9" s="8">
+        <f>SUM(I$3:I9)</f>
         <v>27024</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7">
         <v>999</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B10" s="3" t="s">
+      <c r="H10" s="4"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7">
         <v>525</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="C11" s="9" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8">
-        <f>SUM(E3:E10)</f>
-        <v>27024</v>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8">
+        <f>SUM(F3:F11)</f>
+        <v>27039</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <protectedRanges>
-    <protectedRange sqref="I1:SO504" name="Range1"/>
-    <protectedRange sqref="A11:SH511" name="Range2"/>
-    <protectedRange sqref="F2" name="Range3"/>
-    <protectedRange sqref="F3" name="Range4"/>
-    <protectedRange sqref="F4" name="Range5"/>
-    <protectedRange sqref="F5" name="Range6"/>
-    <protectedRange sqref="F6:F9" name="Range7"/>
-    <protectedRange sqref="F10" name="Range8"/>
+    <protectedRange sqref="J1:SP505" name="Range1"/>
+    <protectedRange sqref="A12:SI512" name="Range2"/>
+    <protectedRange sqref="G2" name="Range3"/>
+    <protectedRange sqref="G3:G4" name="Range4"/>
+    <protectedRange sqref="G5" name="Range5"/>
+    <protectedRange sqref="G6" name="Range6"/>
+    <protectedRange sqref="G7:G10" name="Range7"/>
+    <protectedRange sqref="G11" name="Range8"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>